<commit_message>
cost BOM frame chapes
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/FR/FRA0100_to_FRA0300.xlsx
+++ b/CR - Cost Report/BOM/FR/FRA0100_to_FRA0300.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Cours centrale\EPSA\Optimus\STUF2019\CR - Cost Report\BOM\FR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B8B000-D7A8-47EC-8548-47B4B9FBCD60}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC392A4-82E8-49FD-B9F1-2EE969D0E6DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -351,21 +351,12 @@
     <t>engine bracket</t>
   </si>
   <si>
-    <t>upper PE bracket</t>
-  </si>
-  <si>
-    <t>lower PE bracket</t>
-  </si>
-  <si>
     <t>cooling system bracket</t>
   </si>
   <si>
     <t>fuel tank bracket</t>
   </si>
   <si>
-    <t>chain cover bracket</t>
-  </si>
-  <si>
     <t>pump bracket</t>
   </si>
   <si>
@@ -487,6 +478,15 @@
   </si>
   <si>
     <t>FR_02038</t>
+  </si>
+  <si>
+    <t>chainshield bracket</t>
+  </si>
+  <si>
+    <t>upper excentric carrier bracket</t>
+  </si>
+  <si>
+    <t>lower excentric carrier bracket</t>
   </si>
 </sst>
 </file>
@@ -922,8 +922,8 @@
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E21:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1168,7 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>27</v>
@@ -1249,11 +1249,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>27</v>
@@ -1266,11 +1266,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>27</v>
@@ -1287,7 +1287,7 @@
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>27</v>
@@ -1304,7 +1304,7 @@
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>27</v>
@@ -1321,7 +1321,7 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5" t="s">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>27</v>
@@ -1338,7 +1338,7 @@
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>27</v>
@@ -1355,7 +1355,7 @@
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>27</v>
@@ -1372,7 +1372,7 @@
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>27</v>
@@ -1389,7 +1389,7 @@
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>27</v>
@@ -1406,7 +1406,7 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>27</v>
@@ -1423,7 +1423,7 @@
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>27</v>
@@ -1440,7 +1440,7 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>27</v>
@@ -1457,7 +1457,7 @@
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>27</v>
@@ -1474,7 +1474,7 @@
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>27</v>
@@ -1502,7 +1502,7 @@
         <v>54</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>27</v>
@@ -1519,7 +1519,7 @@
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>27</v>
@@ -1536,7 +1536,7 @@
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>27</v>
@@ -1553,7 +1553,7 @@
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>27</v>
@@ -1570,7 +1570,7 @@
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>27</v>
@@ -1587,7 +1587,7 @@
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>27</v>
@@ -1604,7 +1604,7 @@
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>27</v>
@@ -1621,7 +1621,7 @@
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>27</v>
@@ -1638,7 +1638,7 @@
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>27</v>
@@ -1655,7 +1655,7 @@
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>27</v>
@@ -1680,10 +1680,10 @@
     <row r="44" spans="1:7" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>27</v>
@@ -1712,14 +1712,14 @@
         <v>2</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>27</v>
@@ -1729,14 +1729,14 @@
         <v>6</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>27</v>
@@ -1746,14 +1746,14 @@
         <v>2</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>27</v>
@@ -1763,14 +1763,14 @@
         <v>2</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>27</v>
@@ -1780,14 +1780,14 @@
         <v>4</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>27</v>
@@ -1804,7 +1804,7 @@
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>27</v>
@@ -1821,7 +1821,7 @@
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>27</v>
@@ -1838,7 +1838,7 @@
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>27</v>
@@ -1855,7 +1855,7 @@
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>27</v>
@@ -1872,7 +1872,7 @@
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>27</v>
@@ -1889,7 +1889,7 @@
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>27</v>
@@ -1906,7 +1906,7 @@
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>27</v>
@@ -1923,7 +1923,7 @@
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>27</v>
@@ -1940,7 +1940,7 @@
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>27</v>

</xml_diff>